<commit_message>
Updated Gb_Iu_Planning Template / Fixed minor Bugs Added the possibility to generate several Gb_Iu_Planning at once.
</commit_message>
<xml_diff>
--- a/excel_templates/Gb_Iu_Planning_Template.xlsx
+++ b/excel_templates/Gb_Iu_Planning_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Estudos\core_ps_tool\excel_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProjects\CORE-PS Tool\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -226,7 +226,7 @@
     <definedName name="z" localSheetId="3" hidden="1">{#N/A,#N/A,TRUE,"cover";#N/A,#N/A,TRUE,"contents";#N/A,#N/A,TRUE,"MSC parameters";#N/A,#N/A,TRUE,"Emergency and service numbers";#N/A,#N/A,TRUE,"Charging file parameters";#N/A,#N/A,TRUE,"Charging day classes";#N/A,#N/A,TRUE,"Charging zones";#N/A,#N/A,TRUE,"Change groups";#N/A,#N/A,TRUE,"Signalling links";#N/A,#N/A,TRUE,"Signalling link sets";#N/A,#N/A,TRUE,"Signalling route sets";#N/A,#N/A,TRUE,"GT analysis";#N/A,#N/A,TRUE,"IMSI analysis";#N/A,#N/A,TRUE,"Circuit groups";#N/A,#N/A,TRUE,"Routes";#N/A,#N/A,TRUE,"Number modifications";#N/A,#N/A,TRUE,"Announcements";#N/A,#N/A,TRUE,"Charging cases";#N/A,#N/A,TRUE,"Subdestinations";#N/A,#N/A,TRUE,"Destinations";#N/A,#N/A,TRUE,"Digit analysis";#N/A,#N/A,TRUE,"BTS definitions";#N/A,#N/A,TRUE,"LAC definitions";#N/A,#N/A,TRUE,"BSC definitions"}</definedName>
     <definedName name="z" hidden="1">{#N/A,#N/A,TRUE,"cover";#N/A,#N/A,TRUE,"contents";#N/A,#N/A,TRUE,"MSC parameters";#N/A,#N/A,TRUE,"Emergency and service numbers";#N/A,#N/A,TRUE,"Charging file parameters";#N/A,#N/A,TRUE,"Charging day classes";#N/A,#N/A,TRUE,"Charging zones";#N/A,#N/A,TRUE,"Change groups";#N/A,#N/A,TRUE,"Signalling links";#N/A,#N/A,TRUE,"Signalling link sets";#N/A,#N/A,TRUE,"Signalling route sets";#N/A,#N/A,TRUE,"GT analysis";#N/A,#N/A,TRUE,"IMSI analysis";#N/A,#N/A,TRUE,"Circuit groups";#N/A,#N/A,TRUE,"Routes";#N/A,#N/A,TRUE,"Number modifications";#N/A,#N/A,TRUE,"Announcements";#N/A,#N/A,TRUE,"Charging cases";#N/A,#N/A,TRUE,"Subdestinations";#N/A,#N/A,TRUE,"Destinations";#N/A,#N/A,TRUE,"Digit analysis";#N/A,#N/A,TRUE,"BTS definitions";#N/A,#N/A,TRUE,"LAC definitions";#N/A,#N/A,TRUE,"BSC definitions"}</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1333,19 +1333,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="11">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
-    <numFmt numFmtId="168" formatCode="0.000_)"/>
-    <numFmt numFmtId="169" formatCode="0.00_)"/>
-    <numFmt numFmtId="170" formatCode="[$-416]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="171" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="167" formatCode="0.000_)"/>
+    <numFmt numFmtId="168" formatCode="0.00_)"/>
+    <numFmt numFmtId="169" formatCode="[$-416]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="171" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="69">
     <font>
@@ -1966,7 +1966,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -2548,516 +2548,503 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1289">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="49" fontId="35" fillId="0" borderId="21">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -3090,756 +3077,756 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="29" fillId="29" borderId="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="29" fillId="29" borderId="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="38" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="38" fillId="0" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="38" fillId="0" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="38" fillId="0" borderId="23">
+    <xf numFmtId="166" fontId="38" fillId="0" borderId="23">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="10" fontId="29" fillId="31" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="39" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="37" fontId="40" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="41" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="30" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="29" fillId="30" borderId="1"/>
-    <xf numFmtId="167" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="39" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="29" fillId="30" borderId="1"/>
+    <xf numFmtId="166" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="40" fontId="42" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="43" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="29" fillId="29" borderId="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="38" fillId="0" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="29" fillId="29" borderId="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="38" fillId="0" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="38" fillId="0" borderId="23">
+    <xf numFmtId="166" fontId="38" fillId="0" borderId="23">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="39" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="29" fillId="30" borderId="1"/>
-    <xf numFmtId="167" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="29" fillId="30" borderId="1"/>
+    <xf numFmtId="166" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="169" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="21" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="169" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="16" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="15" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="46" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="46" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="36" fillId="33" borderId="22">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="38" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -3849,39 +3836,39 @@
     <xf numFmtId="0" fontId="48" fillId="29" borderId="6">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="48" fillId="29" borderId="6">
+    <xf numFmtId="170" fontId="48" fillId="29" borderId="6">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
@@ -4008,10 +3995,10 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="118">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="916" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="916" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="916" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="34" borderId="24" xfId="916" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4114,7 +4101,7 @@
     <xf numFmtId="49" fontId="66" fillId="2" borderId="8" xfId="899" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="66" fillId="2" borderId="8" xfId="899" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="66" fillId="2" borderId="8" xfId="899" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="68" fillId="2" borderId="8" xfId="899" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4129,10 +4116,10 @@
     <xf numFmtId="49" fontId="68" fillId="2" borderId="10" xfId="899" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="66" fillId="2" borderId="4" xfId="944" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="66" fillId="2" borderId="4" xfId="944" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="68" fillId="2" borderId="9" xfId="899" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="68" fillId="2" borderId="9" xfId="899" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="34" borderId="35" xfId="916" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4140,48 +4127,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="39" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="39" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="62" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="62" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="62" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="3" borderId="39" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="13" borderId="39" xfId="1285" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="39" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="39" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="13" borderId="43" xfId="1285" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="1285" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4224,10 +4169,52 @@
     <xf numFmtId="0" fontId="59" fillId="2" borderId="16" xfId="1287" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="12" fillId="3" borderId="0" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="12" fillId="3" borderId="0" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="1282" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="13" borderId="39" xfId="1285" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="39" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="39" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="13" borderId="43" xfId="1285" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="62" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="62" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="62" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="39" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="39" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="3" borderId="39" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="3" borderId="44" xfId="1286" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4263,8 +4250,11 @@
     <xf numFmtId="0" fontId="45" fillId="32" borderId="31" xfId="916" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1289">
@@ -5665,9 +5655,9 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Parameters"/>
       <sheetName val="Comments"/>
       <sheetName val="Change Requests"/>
-      <sheetName val="Parameters"/>
       <sheetName val="AdjacentCells"/>
       <sheetName val="Parameters Description"/>
       <sheetName val="AdjacentCells Description"/>
@@ -5676,9 +5666,7 @@
       <sheetName val="Atividade 2_8"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1">
+      <sheetData sheetId="0" refreshError="1">
         <row r="7">
           <cell r="A7">
             <v>50011</v>
@@ -24580,6 +24568,8 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3" refreshError="1"/>
       <sheetData sheetId="4" refreshError="1"/>
       <sheetData sheetId="5" refreshError="1"/>
@@ -24595,8 +24585,8 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="TransSegs"/>
       <sheetName val="VP Routes"/>
-      <sheetName val="TransSegs"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -24954,25 +24944,25 @@
     <row r="3" spans="2:27" ht="62.25" customHeight="1">
       <c r="B3" s="13"/>
       <c r="C3" s="11"/>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
       <c r="I3" s="14"/>
-      <c r="J3" s="104" t="s">
+      <c r="J3" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
-      <c r="Q3" s="104"/>
-      <c r="R3" s="104"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
+      <c r="Q3" s="90"/>
+      <c r="R3" s="90"/>
       <c r="S3" s="11"/>
       <c r="T3" s="15"/>
       <c r="U3" s="11"/>
@@ -24986,25 +24976,25 @@
     <row r="4" spans="2:27" ht="30.75" customHeight="1">
       <c r="B4" s="13"/>
       <c r="C4" s="11"/>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="75"/>
+      <c r="F4" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
       <c r="I4" s="16"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104"/>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
       <c r="S4" s="11"/>
       <c r="T4" s="15"/>
       <c r="U4" s="11"/>
@@ -25018,25 +25008,25 @@
     <row r="5" spans="2:27" ht="30.75" customHeight="1">
       <c r="B5" s="13"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="98"/>
-      <c r="F5" s="99" t="s">
+      <c r="E5" s="84"/>
+      <c r="F5" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
       <c r="I5" s="17"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="104"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="104"/>
-      <c r="Q5" s="104"/>
-      <c r="R5" s="104"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="90"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="90"/>
       <c r="S5" s="11"/>
       <c r="T5" s="15"/>
       <c r="U5" s="11"/>
@@ -25050,21 +25040,21 @@
     <row r="6" spans="2:27" ht="30.75" customHeight="1">
       <c r="B6" s="13"/>
       <c r="C6" s="11"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
       <c r="I6" s="18"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="101"/>
-      <c r="P6" s="101"/>
-      <c r="Q6" s="101"/>
-      <c r="R6" s="101"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
       <c r="S6" s="11"/>
       <c r="T6" s="15"/>
       <c r="U6" s="11"/>
@@ -25078,23 +25068,23 @@
     <row r="7" spans="2:27" ht="30.75" customHeight="1">
       <c r="B7" s="13"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="89" t="s">
+      <c r="D7" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="89"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
       <c r="I7" s="19"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
-      <c r="N7" s="101"/>
-      <c r="O7" s="101"/>
-      <c r="P7" s="101"/>
-      <c r="Q7" s="101"/>
-      <c r="R7" s="101"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
       <c r="S7" s="11"/>
       <c r="T7" s="15"/>
       <c r="U7" s="11"/>
@@ -25108,25 +25098,25 @@
     <row r="8" spans="2:27" ht="30.75" customHeight="1">
       <c r="B8" s="13"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="89" t="s">
+      <c r="D8" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="89"/>
-      <c r="F8" s="103">
+      <c r="E8" s="75"/>
+      <c r="F8" s="89">
         <v>1</v>
       </c>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
       <c r="I8" s="19"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="101"/>
-      <c r="N8" s="101"/>
-      <c r="O8" s="101"/>
-      <c r="P8" s="101"/>
-      <c r="Q8" s="101"/>
-      <c r="R8" s="101"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
       <c r="S8" s="11"/>
       <c r="T8" s="15"/>
       <c r="U8" s="11"/>
@@ -25140,25 +25130,25 @@
     <row r="9" spans="2:27" ht="30.75" customHeight="1" thickBot="1">
       <c r="B9" s="13"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="89" t="s">
+      <c r="D9" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="89"/>
-      <c r="F9" s="90">
+      <c r="E9" s="75"/>
+      <c r="F9" s="76">
         <v>42457</v>
       </c>
-      <c r="G9" s="91"/>
-      <c r="H9" s="91"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
       <c r="I9" s="19"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="102"/>
-      <c r="O9" s="102"/>
-      <c r="P9" s="102"/>
-      <c r="Q9" s="102"/>
-      <c r="R9" s="102"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="88"/>
+      <c r="L9" s="88"/>
+      <c r="M9" s="88"/>
+      <c r="N9" s="88"/>
+      <c r="O9" s="88"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="88"/>
+      <c r="R9" s="88"/>
       <c r="S9" s="11"/>
       <c r="T9" s="15"/>
       <c r="U9" s="11"/>
@@ -25256,25 +25246,25 @@
     <row r="13" spans="2:27" ht="15.75" customHeight="1">
       <c r="B13" s="13"/>
       <c r="C13" s="30"/>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="92"/>
-      <c r="F13" s="92"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
-      <c r="M13" s="93" t="s">
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="N13" s="93"/>
-      <c r="O13" s="93"/>
-      <c r="P13" s="93"/>
-      <c r="Q13" s="93"/>
-      <c r="R13" s="93"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="79"/>
+      <c r="P13" s="79"/>
+      <c r="Q13" s="79"/>
+      <c r="R13" s="79"/>
       <c r="S13" s="34"/>
       <c r="T13" s="15"/>
       <c r="U13" s="11"/>
@@ -25288,27 +25278,27 @@
     <row r="14" spans="2:27" ht="15.75" customHeight="1">
       <c r="B14" s="13"/>
       <c r="C14" s="30"/>
-      <c r="D14" s="94" t="s">
+      <c r="D14" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="95" t="s">
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="95"/>
-      <c r="J14" s="95"/>
-      <c r="K14" s="95"/>
-      <c r="L14" s="95"/>
-      <c r="M14" s="96" t="s">
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="N14" s="96"/>
-      <c r="O14" s="96"/>
-      <c r="P14" s="96"/>
-      <c r="Q14" s="96"/>
-      <c r="R14" s="96"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="82"/>
       <c r="S14" s="34"/>
       <c r="T14" s="15"/>
       <c r="U14" s="11"/>
@@ -25322,27 +25312,27 @@
     <row r="15" spans="2:27" ht="15.75" customHeight="1">
       <c r="B15" s="13"/>
       <c r="C15" s="30"/>
-      <c r="D15" s="85" t="s">
+      <c r="D15" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="85"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86" t="s">
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
-      <c r="L15" s="86"/>
-      <c r="M15" s="87" t="s">
+      <c r="I15" s="95"/>
+      <c r="J15" s="95"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="95"/>
+      <c r="M15" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="N15" s="87"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="87"/>
-      <c r="R15" s="87"/>
+      <c r="N15" s="96"/>
+      <c r="O15" s="96"/>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="96"/>
+      <c r="R15" s="96"/>
       <c r="S15" s="34"/>
       <c r="T15" s="15"/>
       <c r="U15" s="11"/>
@@ -25469,29 +25459,29 @@
     <row r="20" spans="2:27" ht="15.75" customHeight="1">
       <c r="B20" s="13"/>
       <c r="C20" s="30"/>
-      <c r="D20" s="88" t="s">
+      <c r="D20" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88" t="s">
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88" t="s">
+      <c r="I20" s="97"/>
+      <c r="J20" s="97"/>
+      <c r="K20" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="L20" s="88"/>
-      <c r="M20" s="88" t="s">
+      <c r="L20" s="97"/>
+      <c r="M20" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="N20" s="88"/>
-      <c r="O20" s="88"/>
-      <c r="P20" s="88"/>
-      <c r="Q20" s="88"/>
-      <c r="R20" s="88"/>
+      <c r="N20" s="97"/>
+      <c r="O20" s="97"/>
+      <c r="P20" s="97"/>
+      <c r="Q20" s="97"/>
+      <c r="R20" s="97"/>
       <c r="S20" s="34"/>
       <c r="T20" s="15"/>
       <c r="U20" s="11"/>
@@ -25505,21 +25495,21 @@
     <row r="21" spans="2:27" ht="15">
       <c r="B21" s="13"/>
       <c r="C21" s="30"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="84"/>
-      <c r="K21" s="77"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="78"/>
-      <c r="N21" s="77"/>
-      <c r="O21" s="77"/>
-      <c r="P21" s="77"/>
-      <c r="Q21" s="77"/>
-      <c r="R21" s="77"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="92"/>
+      <c r="I21" s="92"/>
+      <c r="J21" s="92"/>
+      <c r="K21" s="91"/>
+      <c r="L21" s="91"/>
+      <c r="M21" s="93"/>
+      <c r="N21" s="91"/>
+      <c r="O21" s="91"/>
+      <c r="P21" s="91"/>
+      <c r="Q21" s="91"/>
+      <c r="R21" s="91"/>
       <c r="S21" s="34"/>
       <c r="T21" s="15"/>
       <c r="U21" s="11"/>
@@ -25533,21 +25523,21 @@
     <row r="22" spans="2:27" ht="15">
       <c r="B22" s="13"/>
       <c r="C22" s="30"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="77"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="84"/>
-      <c r="K22" s="77"/>
-      <c r="L22" s="77"/>
-      <c r="M22" s="78"/>
-      <c r="N22" s="77"/>
-      <c r="O22" s="77"/>
-      <c r="P22" s="77"/>
-      <c r="Q22" s="77"/>
-      <c r="R22" s="77"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="92"/>
+      <c r="K22" s="91"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="93"/>
+      <c r="N22" s="91"/>
+      <c r="O22" s="91"/>
+      <c r="P22" s="91"/>
+      <c r="Q22" s="91"/>
+      <c r="R22" s="91"/>
       <c r="S22" s="34"/>
       <c r="T22" s="15"/>
       <c r="U22" s="11"/>
@@ -25561,21 +25551,21 @@
     <row r="23" spans="2:27" ht="15">
       <c r="B23" s="13"/>
       <c r="C23" s="30"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="78"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="77"/>
-      <c r="P23" s="77"/>
-      <c r="Q23" s="77"/>
-      <c r="R23" s="77"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="91"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="92"/>
+      <c r="J23" s="92"/>
+      <c r="K23" s="91"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="93"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="91"/>
+      <c r="P23" s="91"/>
+      <c r="Q23" s="91"/>
+      <c r="R23" s="91"/>
       <c r="S23" s="34"/>
       <c r="T23" s="15"/>
       <c r="U23" s="11"/>
@@ -25589,21 +25579,21 @@
     <row r="24" spans="2:27" ht="15">
       <c r="B24" s="13"/>
       <c r="C24" s="30"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="84"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="78"/>
-      <c r="N24" s="77"/>
-      <c r="O24" s="77"/>
-      <c r="P24" s="77"/>
-      <c r="Q24" s="77"/>
-      <c r="R24" s="77"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="91"/>
+      <c r="G24" s="91"/>
+      <c r="H24" s="92"/>
+      <c r="I24" s="92"/>
+      <c r="J24" s="92"/>
+      <c r="K24" s="91"/>
+      <c r="L24" s="91"/>
+      <c r="M24" s="93"/>
+      <c r="N24" s="91"/>
+      <c r="O24" s="91"/>
+      <c r="P24" s="91"/>
+      <c r="Q24" s="91"/>
+      <c r="R24" s="91"/>
       <c r="S24" s="34"/>
       <c r="T24" s="15"/>
       <c r="U24" s="11"/>
@@ -25617,21 +25607,21 @@
     <row r="25" spans="2:27" ht="15">
       <c r="B25" s="13"/>
       <c r="C25" s="30"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="84"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="78"/>
-      <c r="N25" s="78"/>
-      <c r="O25" s="78"/>
-      <c r="P25" s="78"/>
-      <c r="Q25" s="78"/>
-      <c r="R25" s="78"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="91"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="91"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="93"/>
+      <c r="N25" s="93"/>
+      <c r="O25" s="93"/>
+      <c r="P25" s="93"/>
+      <c r="Q25" s="93"/>
+      <c r="R25" s="93"/>
       <c r="S25" s="34"/>
       <c r="T25" s="15"/>
       <c r="U25" s="11"/>
@@ -25645,21 +25635,21 @@
     <row r="26" spans="2:27" ht="15">
       <c r="B26" s="13"/>
       <c r="C26" s="30"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="79"/>
-      <c r="L26" s="79"/>
-      <c r="M26" s="81"/>
-      <c r="N26" s="81"/>
-      <c r="O26" s="81"/>
-      <c r="P26" s="81"/>
-      <c r="Q26" s="81"/>
-      <c r="R26" s="81"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="99"/>
+      <c r="I26" s="99"/>
+      <c r="J26" s="99"/>
+      <c r="K26" s="98"/>
+      <c r="L26" s="98"/>
+      <c r="M26" s="100"/>
+      <c r="N26" s="100"/>
+      <c r="O26" s="100"/>
+      <c r="P26" s="100"/>
+      <c r="Q26" s="100"/>
+      <c r="R26" s="100"/>
       <c r="S26" s="34"/>
       <c r="T26" s="15"/>
       <c r="U26" s="11"/>
@@ -25673,21 +25663,21 @@
     <row r="27" spans="2:27" ht="15">
       <c r="B27" s="13"/>
       <c r="C27" s="30"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
-      <c r="M27" s="81"/>
-      <c r="N27" s="81"/>
-      <c r="O27" s="81"/>
-      <c r="P27" s="81"/>
-      <c r="Q27" s="81"/>
-      <c r="R27" s="81"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="99"/>
+      <c r="I27" s="99"/>
+      <c r="J27" s="99"/>
+      <c r="K27" s="98"/>
+      <c r="L27" s="98"/>
+      <c r="M27" s="100"/>
+      <c r="N27" s="100"/>
+      <c r="O27" s="100"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="100"/>
+      <c r="R27" s="100"/>
       <c r="S27" s="34"/>
       <c r="T27" s="15"/>
       <c r="U27" s="11"/>
@@ -25701,21 +25691,21 @@
     <row r="28" spans="2:27" ht="15">
       <c r="B28" s="13"/>
       <c r="C28" s="30"/>
-      <c r="D28" s="79"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="79"/>
-      <c r="M28" s="81"/>
-      <c r="N28" s="81"/>
-      <c r="O28" s="81"/>
-      <c r="P28" s="81"/>
-      <c r="Q28" s="81"/>
-      <c r="R28" s="81"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="99"/>
+      <c r="J28" s="99"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="98"/>
+      <c r="M28" s="100"/>
+      <c r="N28" s="100"/>
+      <c r="O28" s="100"/>
+      <c r="P28" s="100"/>
+      <c r="Q28" s="100"/>
+      <c r="R28" s="100"/>
       <c r="S28" s="34"/>
       <c r="T28" s="15"/>
       <c r="U28" s="11"/>
@@ -25729,21 +25719,21 @@
     <row r="29" spans="2:27" ht="15">
       <c r="B29" s="13"/>
       <c r="C29" s="30"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="80"/>
-      <c r="K29" s="79"/>
-      <c r="L29" s="79"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="81"/>
-      <c r="O29" s="81"/>
-      <c r="P29" s="81"/>
-      <c r="Q29" s="81"/>
-      <c r="R29" s="81"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="98"/>
+      <c r="G29" s="98"/>
+      <c r="H29" s="99"/>
+      <c r="I29" s="99"/>
+      <c r="J29" s="99"/>
+      <c r="K29" s="98"/>
+      <c r="L29" s="98"/>
+      <c r="M29" s="100"/>
+      <c r="N29" s="100"/>
+      <c r="O29" s="100"/>
+      <c r="P29" s="100"/>
+      <c r="Q29" s="100"/>
+      <c r="R29" s="100"/>
       <c r="S29" s="34"/>
       <c r="T29" s="15"/>
       <c r="U29" s="11"/>
@@ -25757,21 +25747,21 @@
     <row r="30" spans="2:27" ht="15">
       <c r="B30" s="13"/>
       <c r="C30" s="30"/>
-      <c r="D30" s="79"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="80"/>
-      <c r="I30" s="80"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="79"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="81"/>
-      <c r="N30" s="81"/>
-      <c r="O30" s="81"/>
-      <c r="P30" s="81"/>
-      <c r="Q30" s="81"/>
-      <c r="R30" s="81"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="99"/>
+      <c r="I30" s="99"/>
+      <c r="J30" s="99"/>
+      <c r="K30" s="98"/>
+      <c r="L30" s="98"/>
+      <c r="M30" s="100"/>
+      <c r="N30" s="100"/>
+      <c r="O30" s="100"/>
+      <c r="P30" s="100"/>
+      <c r="Q30" s="100"/>
+      <c r="R30" s="100"/>
       <c r="S30" s="34"/>
       <c r="T30" s="15"/>
       <c r="U30" s="11"/>
@@ -25785,21 +25775,21 @@
     <row r="31" spans="2:27" ht="15">
       <c r="B31" s="13"/>
       <c r="C31" s="30"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="80"/>
-      <c r="I31" s="80"/>
-      <c r="J31" s="80"/>
-      <c r="K31" s="79"/>
-      <c r="L31" s="79"/>
-      <c r="M31" s="81"/>
-      <c r="N31" s="81"/>
-      <c r="O31" s="81"/>
-      <c r="P31" s="81"/>
-      <c r="Q31" s="81"/>
-      <c r="R31" s="81"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="99"/>
+      <c r="I31" s="99"/>
+      <c r="J31" s="99"/>
+      <c r="K31" s="98"/>
+      <c r="L31" s="98"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="100"/>
+      <c r="Q31" s="100"/>
+      <c r="R31" s="100"/>
       <c r="S31" s="34"/>
       <c r="T31" s="15"/>
       <c r="U31" s="11"/>
@@ -25813,21 +25803,21 @@
     <row r="32" spans="2:27" ht="15">
       <c r="B32" s="13"/>
       <c r="C32" s="30"/>
-      <c r="D32" s="79"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="79"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="80"/>
-      <c r="K32" s="79"/>
-      <c r="L32" s="79"/>
-      <c r="M32" s="81"/>
-      <c r="N32" s="81"/>
-      <c r="O32" s="81"/>
-      <c r="P32" s="81"/>
-      <c r="Q32" s="81"/>
-      <c r="R32" s="81"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="99"/>
+      <c r="I32" s="99"/>
+      <c r="J32" s="99"/>
+      <c r="K32" s="98"/>
+      <c r="L32" s="98"/>
+      <c r="M32" s="100"/>
+      <c r="N32" s="100"/>
+      <c r="O32" s="100"/>
+      <c r="P32" s="100"/>
+      <c r="Q32" s="100"/>
+      <c r="R32" s="100"/>
       <c r="S32" s="34"/>
       <c r="T32" s="15"/>
       <c r="U32" s="11"/>
@@ -25841,21 +25831,21 @@
     <row r="33" spans="2:27" ht="15">
       <c r="B33" s="13"/>
       <c r="C33" s="30"/>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="80"/>
-      <c r="I33" s="80"/>
-      <c r="J33" s="80"/>
-      <c r="K33" s="79"/>
-      <c r="L33" s="79"/>
-      <c r="M33" s="81"/>
-      <c r="N33" s="81"/>
-      <c r="O33" s="81"/>
-      <c r="P33" s="81"/>
-      <c r="Q33" s="81"/>
-      <c r="R33" s="81"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="98"/>
+      <c r="G33" s="98"/>
+      <c r="H33" s="99"/>
+      <c r="I33" s="99"/>
+      <c r="J33" s="99"/>
+      <c r="K33" s="98"/>
+      <c r="L33" s="98"/>
+      <c r="M33" s="100"/>
+      <c r="N33" s="100"/>
+      <c r="O33" s="100"/>
+      <c r="P33" s="100"/>
+      <c r="Q33" s="100"/>
+      <c r="R33" s="100"/>
       <c r="S33" s="34"/>
       <c r="T33" s="15"/>
       <c r="U33" s="11"/>
@@ -25869,21 +25859,21 @@
     <row r="34" spans="2:27" ht="15">
       <c r="B34" s="13"/>
       <c r="C34" s="30"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="80"/>
-      <c r="I34" s="80"/>
-      <c r="J34" s="80"/>
-      <c r="K34" s="79"/>
-      <c r="L34" s="79"/>
-      <c r="M34" s="81"/>
-      <c r="N34" s="81"/>
-      <c r="O34" s="81"/>
-      <c r="P34" s="81"/>
-      <c r="Q34" s="81"/>
-      <c r="R34" s="81"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="99"/>
+      <c r="I34" s="99"/>
+      <c r="J34" s="99"/>
+      <c r="K34" s="98"/>
+      <c r="L34" s="98"/>
+      <c r="M34" s="100"/>
+      <c r="N34" s="100"/>
+      <c r="O34" s="100"/>
+      <c r="P34" s="100"/>
+      <c r="Q34" s="100"/>
+      <c r="R34" s="100"/>
       <c r="S34" s="34"/>
       <c r="T34" s="15"/>
       <c r="U34" s="11"/>
@@ -25897,21 +25887,21 @@
     <row r="35" spans="2:27" ht="15">
       <c r="B35" s="13"/>
       <c r="C35" s="30"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="81"/>
-      <c r="N35" s="81"/>
-      <c r="O35" s="81"/>
-      <c r="P35" s="81"/>
-      <c r="Q35" s="81"/>
-      <c r="R35" s="81"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="99"/>
+      <c r="J35" s="99"/>
+      <c r="K35" s="98"/>
+      <c r="L35" s="98"/>
+      <c r="M35" s="100"/>
+      <c r="N35" s="100"/>
+      <c r="O35" s="100"/>
+      <c r="P35" s="100"/>
+      <c r="Q35" s="100"/>
+      <c r="R35" s="100"/>
       <c r="S35" s="34"/>
       <c r="T35" s="15"/>
       <c r="U35" s="11"/>
@@ -25925,21 +25915,21 @@
     <row r="36" spans="2:27" ht="15">
       <c r="B36" s="13"/>
       <c r="C36" s="30"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="82"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="82"/>
-      <c r="H36" s="82"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="82"/>
-      <c r="K36" s="82"/>
-      <c r="L36" s="82"/>
-      <c r="M36" s="83"/>
-      <c r="N36" s="83"/>
-      <c r="O36" s="83"/>
-      <c r="P36" s="83"/>
-      <c r="Q36" s="83"/>
-      <c r="R36" s="83"/>
+      <c r="D36" s="103"/>
+      <c r="E36" s="103"/>
+      <c r="F36" s="103"/>
+      <c r="G36" s="103"/>
+      <c r="H36" s="103"/>
+      <c r="I36" s="103"/>
+      <c r="J36" s="103"/>
+      <c r="K36" s="103"/>
+      <c r="L36" s="103"/>
+      <c r="M36" s="104"/>
+      <c r="N36" s="104"/>
+      <c r="O36" s="104"/>
+      <c r="P36" s="104"/>
+      <c r="Q36" s="104"/>
+      <c r="R36" s="104"/>
       <c r="S36" s="34"/>
       <c r="T36" s="15"/>
       <c r="U36" s="11"/>
@@ -25953,21 +25943,21 @@
     <row r="37" spans="2:27" ht="15">
       <c r="B37" s="13"/>
       <c r="C37" s="30"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="75"/>
-      <c r="J37" s="75"/>
-      <c r="K37" s="75"/>
-      <c r="L37" s="75"/>
-      <c r="M37" s="76"/>
-      <c r="N37" s="75"/>
-      <c r="O37" s="75"/>
-      <c r="P37" s="75"/>
-      <c r="Q37" s="75"/>
-      <c r="R37" s="75"/>
+      <c r="D37" s="101"/>
+      <c r="E37" s="101"/>
+      <c r="F37" s="101"/>
+      <c r="G37" s="101"/>
+      <c r="H37" s="101"/>
+      <c r="I37" s="101"/>
+      <c r="J37" s="101"/>
+      <c r="K37" s="101"/>
+      <c r="L37" s="101"/>
+      <c r="M37" s="102"/>
+      <c r="N37" s="101"/>
+      <c r="O37" s="101"/>
+      <c r="P37" s="101"/>
+      <c r="Q37" s="101"/>
+      <c r="R37" s="101"/>
       <c r="S37" s="34"/>
       <c r="T37" s="15"/>
       <c r="U37" s="11"/>
@@ -25981,21 +25971,21 @@
     <row r="38" spans="2:27" ht="15">
       <c r="B38" s="13"/>
       <c r="C38" s="30"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="75"/>
-      <c r="I38" s="75"/>
-      <c r="J38" s="75"/>
-      <c r="K38" s="75"/>
-      <c r="L38" s="75"/>
-      <c r="M38" s="76"/>
-      <c r="N38" s="75"/>
-      <c r="O38" s="75"/>
-      <c r="P38" s="75"/>
-      <c r="Q38" s="75"/>
-      <c r="R38" s="75"/>
+      <c r="D38" s="101"/>
+      <c r="E38" s="101"/>
+      <c r="F38" s="101"/>
+      <c r="G38" s="101"/>
+      <c r="H38" s="101"/>
+      <c r="I38" s="101"/>
+      <c r="J38" s="101"/>
+      <c r="K38" s="101"/>
+      <c r="L38" s="101"/>
+      <c r="M38" s="102"/>
+      <c r="N38" s="101"/>
+      <c r="O38" s="101"/>
+      <c r="P38" s="101"/>
+      <c r="Q38" s="101"/>
+      <c r="R38" s="101"/>
       <c r="S38" s="34"/>
       <c r="T38" s="15"/>
       <c r="U38" s="11"/>
@@ -26009,21 +25999,21 @@
     <row r="39" spans="2:27" ht="15">
       <c r="B39" s="13"/>
       <c r="C39" s="30"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="77"/>
-      <c r="I39" s="77"/>
-      <c r="J39" s="77"/>
-      <c r="K39" s="77"/>
-      <c r="L39" s="77"/>
-      <c r="M39" s="78"/>
-      <c r="N39" s="77"/>
-      <c r="O39" s="77"/>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="77"/>
-      <c r="R39" s="77"/>
+      <c r="D39" s="91"/>
+      <c r="E39" s="91"/>
+      <c r="F39" s="91"/>
+      <c r="G39" s="91"/>
+      <c r="H39" s="91"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="91"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="91"/>
+      <c r="M39" s="93"/>
+      <c r="N39" s="91"/>
+      <c r="O39" s="91"/>
+      <c r="P39" s="91"/>
+      <c r="Q39" s="91"/>
+      <c r="R39" s="91"/>
       <c r="S39" s="34"/>
       <c r="T39" s="15"/>
       <c r="U39" s="11"/>
@@ -26037,21 +26027,21 @@
     <row r="40" spans="2:27" ht="15">
       <c r="B40" s="13"/>
       <c r="C40" s="30"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="77"/>
-      <c r="G40" s="77"/>
-      <c r="H40" s="77"/>
-      <c r="I40" s="77"/>
-      <c r="J40" s="77"/>
-      <c r="K40" s="77"/>
-      <c r="L40" s="77"/>
-      <c r="M40" s="78"/>
-      <c r="N40" s="77"/>
-      <c r="O40" s="77"/>
-      <c r="P40" s="77"/>
-      <c r="Q40" s="77"/>
-      <c r="R40" s="77"/>
+      <c r="D40" s="91"/>
+      <c r="E40" s="91"/>
+      <c r="F40" s="91"/>
+      <c r="G40" s="91"/>
+      <c r="H40" s="91"/>
+      <c r="I40" s="91"/>
+      <c r="J40" s="91"/>
+      <c r="K40" s="91"/>
+      <c r="L40" s="91"/>
+      <c r="M40" s="93"/>
+      <c r="N40" s="91"/>
+      <c r="O40" s="91"/>
+      <c r="P40" s="91"/>
+      <c r="Q40" s="91"/>
+      <c r="R40" s="91"/>
       <c r="S40" s="34"/>
       <c r="T40" s="15"/>
       <c r="U40" s="11"/>
@@ -26065,21 +26055,21 @@
     <row r="41" spans="2:27" ht="15">
       <c r="B41" s="13"/>
       <c r="C41" s="30"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
-      <c r="M41" s="76"/>
-      <c r="N41" s="75"/>
-      <c r="O41" s="75"/>
-      <c r="P41" s="75"/>
-      <c r="Q41" s="75"/>
-      <c r="R41" s="75"/>
+      <c r="D41" s="101"/>
+      <c r="E41" s="101"/>
+      <c r="F41" s="101"/>
+      <c r="G41" s="101"/>
+      <c r="H41" s="101"/>
+      <c r="I41" s="101"/>
+      <c r="J41" s="101"/>
+      <c r="K41" s="101"/>
+      <c r="L41" s="101"/>
+      <c r="M41" s="102"/>
+      <c r="N41" s="101"/>
+      <c r="O41" s="101"/>
+      <c r="P41" s="101"/>
+      <c r="Q41" s="101"/>
+      <c r="R41" s="101"/>
       <c r="S41" s="34"/>
       <c r="T41" s="15"/>
       <c r="U41" s="11"/>
@@ -26281,6 +26271,97 @@
     <protectedRange sqref="E23" name="General Topology_1_1_1" securityDescriptor="O:WDG:WDD:(A;;CC;;;WD)"/>
   </protectedRanges>
   <mergeCells count="110">
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="M41:R41"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="M39:R39"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="M40:R40"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:R37"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="M38:R38"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="M35:R35"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:R36"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:R33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:R34"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:R31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:R32"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:R30"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:R27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:R28"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:R25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:R26"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:R23"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:R24"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:R21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:R22"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="M15:R15"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:R20"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="D13:G13"/>
@@ -26300,97 +26381,6 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="J3:R5"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:R21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:R22"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="M15:R15"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:R20"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:R25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:R26"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:R23"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:R24"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:R29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:R30"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:R27"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:R28"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:R33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:R34"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:R31"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:R32"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:R37"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="M38:R38"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="M35:R35"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:R36"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="M41:R41"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="M39:R39"/>
-    <mergeCell ref="D40:G40"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="M40:R40"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="3">
@@ -26410,10 +26400,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
@@ -26450,7 +26440,7 @@
       <c r="L1" s="108"/>
       <c r="M1" s="109"/>
     </row>
-    <row r="2" spans="1:13" ht="38.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="116" t="s">
         <v>14</v>
       </c>
@@ -26491,10 +26481,38 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="117"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="15">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:M1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>